<commit_message>
School Address Info added
</commit_message>
<xml_diff>
--- a/requirements.xlsx
+++ b/requirements.xlsx
@@ -83,6 +83,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Pending Sales/</t>
     </r>
     <r>
@@ -1914,9 +1921,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2250,8 +2258,8 @@
   <sheetPr/>
   <dimension ref="B1:F188"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="C21" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -2267,7 +2275,7 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
@@ -2338,7 +2346,7 @@
       <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2414,13 +2422,13 @@
       <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2969,19 +2977,19 @@
       </c>
     </row>
     <row r="54" s="1" customFormat="1" spans="2:6">
-      <c r="B54" s="2">
+      <c r="B54" s="3">
         <v>42</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E54" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F54" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3002,20 +3010,20 @@
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="2:6">
-      <c r="B56">
+    <row r="56" s="2" customFormat="1" spans="2:6">
+      <c r="B56" s="2">
         <v>44</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="3" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3623,7 +3631,7 @@
       <c r="E104" t="s">
         <v>41</v>
       </c>
-      <c r="F104" s="7" t="s">
+      <c r="F104" s="8" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3641,17 +3649,17 @@
         <v>117</v>
       </c>
     </row>
-    <row r="106" s="2" customFormat="1" spans="2:6">
-      <c r="B106" s="2">
+    <row r="106" s="3" customFormat="1" spans="2:6">
+      <c r="B106" s="3">
         <v>81</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="D106" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E106" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F106" s="2" t="s">
+      <c r="E106" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F106" s="3" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
School Value Statements, School Engagement Activities, Sales Documentation, Field Technical Checklist, Remote Technical Checklist added
</commit_message>
<xml_diff>
--- a/requirements.xlsx
+++ b/requirements.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="218">
   <si>
     <t>Mandatory</t>
   </si>
@@ -1921,10 +1921,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2258,8 +2257,8 @@
   <sheetPr/>
   <dimension ref="B1:F188"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -2275,7 +2274,7 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
@@ -2346,7 +2345,7 @@
       <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2422,13 +2421,13 @@
       <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2977,19 +2976,19 @@
       </c>
     </row>
     <row r="54" s="1" customFormat="1" spans="2:6">
-      <c r="B54" s="3">
+      <c r="B54" s="2">
         <v>42</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="F54" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3014,16 +3013,16 @@
       <c r="B56" s="2">
         <v>44</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F56" s="2" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3631,7 +3630,7 @@
       <c r="E104" t="s">
         <v>41</v>
       </c>
-      <c r="F104" s="8" t="s">
+      <c r="F104" s="7" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3649,17 +3648,17 @@
         <v>117</v>
       </c>
     </row>
-    <row r="106" s="3" customFormat="1" spans="2:6">
-      <c r="B106" s="3">
+    <row r="106" s="2" customFormat="1" spans="2:6">
+      <c r="B106" s="2">
         <v>81</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="D106" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E106" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F106" s="3" t="s">
+      <c r="E106" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F106" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3743,7 +3742,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="115" spans="2:6">
+    <row r="115" spans="2:5">
       <c r="B115">
         <v>87</v>
       </c>
@@ -3752,9 +3751,6 @@
       </c>
       <c r="E115" t="s">
         <v>20</v>
-      </c>
-      <c r="F115" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="116" spans="2:5">

</xml_diff>